<commit_message>
Upated README and images
</commit_message>
<xml_diff>
--- a/images/BERT Performance.xlsx
+++ b/images/BERT Performance.xlsx
@@ -5,54 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothy/Documents/Github/bert-finetune/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488D6CD3-5A5E-F345-9771-9AA38BFBA007}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A943F27-422A-4A4B-A3A9-A7E06DC7B957}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8B8067C8-0296-5D4C-86C0-A9E7EAFB1B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$5:$A$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$5:$B$7</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$5:$A$7</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$5:$B$7</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$A$5:$A$7</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$B$5:$B$7</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$A$17</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$A$30</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$30:$E$30</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$17</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$17</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$A$30</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$B$30:$E$30</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$A$17</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$A$18</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$30</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$B$35:$E$35</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$A$17</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$A$30</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$B$30:$E$30</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$30:$E$30</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$33:$E$33</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$34:$E$34</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$17</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$30</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$30:$E$30</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1736,7 +1698,7 @@
               <a:rPr lang="en-GB" sz="1600" b="0" i="0">
                 <a:latin typeface="DINPro Medium" panose="02000503030000020004" pitchFamily="2" charset="0"/>
               </a:rPr>
-              <a:t>Fine-tuning BERTBASE</a:t>
+              <a:t>Fine-tuning BERTLARGE</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2722,7 +2684,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2967,6 +2929,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1695621503"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -7552,8 +7515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E751DE-BC54-3740-8EFA-CD1A254CABDE}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>